<commit_message>
- Added email notification - Created HTML template for email
</commit_message>
<xml_diff>
--- a/output/publications.xlsx
+++ b/output/publications.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:D4"/>
@@ -486,523 +486,843 @@
       <c r="D2" s="2" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Wind speed influence on phytoplankton bloom dynamics in the Southern Ocean Marginal Ice Zone</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t>Dillon T Fitch and J Keith Moore</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="2" t="inlineStr">
         <is>
           <t>https://agupubs.onlinelibrary.wiley.com/doi/abs/10.1029/2006JC004061</t>
         </is>
       </c>
-      <c r="D3" t="n">
+      <c r="D3" s="2" t="n">
         <v>2007</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>Traffic stress and bicycling to elementary and junior high school: Evidence from Davis, California</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>Dillon Fitch and Calvin Thigpen and Susan Handy</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="2" t="inlineStr">
         <is>
           <t>https://www.sciencedirect.com/science/article/pii/S2214140516000098</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="D4" s="2" t="n">
         <v>2015</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>How the built environment affects physical activity: views from urban planning</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="2" t="inlineStr">
         <is>
           <t>Susan L Handy and Marlon G Boarnet and Reid Ewing and Richard E Killingsworth</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>https://www.sciencedirect.com/science/article/pii/S0749379702004750</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="D5" s="2" t="n">
         <v>2002</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>Built environment correlates of walking: a review</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t>Brian E Saelens and Susan L Handy</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="2" t="inlineStr">
         <is>
           <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC2921187/</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="D6" s="2" t="n">
         <v>2008</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>Network robustness index: A new method for identifying critical links and evaluating the performance of transportation networks</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>Darren M Scott and David C Novak and Lisa Aultman-Hall and Feng Guo</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="2" t="inlineStr">
         <is>
           <t>https://www.sciencedirect.com/science/article/pii/S0966692305000694</t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="D7" s="2" t="n">
         <v>2006</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="2" t="inlineStr">
         <is>
           <t>Identifying critical road segments and measuring system-wide robustness in transportation networks with isolating links: A link-based capacity-reduction approach</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="2" t="inlineStr">
         <is>
           <t>James L Sullivan and David C Novak and Lisa Aultman-Hall and David M Scott</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" s="2" t="inlineStr">
         <is>
           <t>https://www.sciencedirect.com/science/article/pii/S0965856410000418</t>
         </is>
       </c>
-      <c r="D8" t="n">
+      <c r="D8" s="2" t="n">
         <v>2010</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr">
         <is>
           <t>Neighborhood change, one pint at a time: The impact of local characteristics on craft breweries</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="2" t="inlineStr">
         <is>
           <t>Jesus M Barajas and Geoff Boeing and Julie Wartell</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="2" t="inlineStr">
         <is>
           <t>https://papers.ssrn.com/Sol3/papers.cfm?abstract_id=2936427</t>
         </is>
       </c>
-      <c r="D9" t="n">
+      <c r="D9" s="2" t="n">
         <v>2017</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="2" t="inlineStr">
         <is>
           <t>Supplemental infrastructure: how community networks and immigrant identity influence cycling</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="2" t="inlineStr">
         <is>
           <t>Jesus M Barajas</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" s="2" t="inlineStr">
         <is>
           <t>https://link.springer.com/article/10.1007/s11116-018-9955-7</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="D10" s="2" t="n">
         <v>2020</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>What influences travelers to use Uber? Exploring the factors affecting the adoption of on-demand ride services in California</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="2" t="inlineStr">
         <is>
           <t>Farzad Alemi and Giovanni Circella and Susan Handy and Patricia Mokhtarian</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" s="2" t="inlineStr">
         <is>
           <t>https://www.sciencedirect.com/science/article/pii/S2214367X17300947</t>
         </is>
       </c>
-      <c r="D11" t="n">
+      <c r="D11" s="2" t="n">
         <v>2018</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="2" t="inlineStr">
         <is>
           <t>How do activities conducted while commuting influence mode choice? Using revealed preference models to inform public transportation advantage and autonomous vehicle scenarios</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" s="2" t="inlineStr">
         <is>
           <t>Aliaksandr Malokin and Giovanni Circella and Patricia L Mokhtarian</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>https://www.sciencedirect.com/science/article/pii/S0965856416306772</t>
         </is>
       </c>
-      <c r="D12" t="n">
+      <c r="D12" s="2" t="n">
         <v>2019</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="2" t="inlineStr">
         <is>
           <t>Olympic technologies: Tokyo 2020 and beyond: the urban technology metropolis</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="2" t="inlineStr">
         <is>
           <t>Eva Kassens-Noor and Tatsuya Fukushige</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="2" t="inlineStr">
         <is>
           <t>https://www.tandfonline.com/doi/abs/10.1080/10630732.2016.1157949</t>
         </is>
       </c>
-      <c r="D13" t="n">
+      <c r="D13" s="2" t="n">
         <v>2018</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="2" t="inlineStr">
         <is>
           <t>Factors influencing dock-less E-bike-share mode substitution: Evidence from Sacramento, California</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" s="2" t="inlineStr">
         <is>
           <t>Tatsuya Fukushige and Dillon T Fitch and Susan Handy</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" s="2" t="inlineStr">
         <is>
           <t>https://www.sciencedirect.com/science/article/pii/S1361920921002881</t>
         </is>
       </c>
-      <c r="D14" t="n">
+      <c r="D14" s="2" t="n">
         <v>2021</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="2" t="inlineStr">
         <is>
           <t>On the unique features of post-disaster humanitarian logistics</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" s="2" t="inlineStr">
         <is>
           <t>José Holguín-Veras and Miguel Jaller and Luk N Van Wassenhove and Noel Pérez and Tricia Wachtendorf</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" s="2" t="inlineStr">
         <is>
           <t>https://www.sciencedirect.com/science/article/pii/S0272696312000654</t>
         </is>
       </c>
-      <c r="D15" t="n">
+      <c r="D15" s="2" t="n">
         <v>2012</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="2" t="inlineStr">
         <is>
           <t>On the appropriate objective function for post-disaster humanitarian logistics models</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" s="2" t="inlineStr">
         <is>
           <t>José Holguín-Veras and Noel Pérez and Miguel Jaller and Luk N Van Wassenhove and Felipe Aros-Vera</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C16" s="2" t="inlineStr">
         <is>
           <t>https://www.sciencedirect.com/science/article/pii/S0272696313000417</t>
         </is>
       </c>
-      <c r="D16" t="n">
+      <c r="D16" s="2" t="n">
         <v>2013</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="2" t="inlineStr">
         <is>
           <t>A subpopulation of macrophages infiltrates hypertrophic adipose tissue and is activated by free fatty acids via Toll-like receptors 2 and 4 and JNK-dependent pathways</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" s="2" t="inlineStr">
         <is>
           <t>MT Audrey Nguyen and Svetlana Favelyukis and Anh-Khoi Nguyen and Donna Reichart and Peter A Scott and Alan Jenn and Ru Liu-Bryan and Christopher K Glass and Jaap G Neels and Jerrold M Olefsky</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C17" s="2" t="inlineStr">
         <is>
           <t>https://www.jbc.org/article/S0021-9258(20)54665-6/abstract</t>
         </is>
       </c>
-      <c r="D17" t="n">
+      <c r="D17" s="2" t="n">
         <v>2007</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="2" t="inlineStr">
         <is>
           <t>A review of consumer preferences of and interactions with electric vehicle charging infrastructure</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" s="2" t="inlineStr">
         <is>
           <t>Scott Hardman and Alan Jenn and Gil Tal and Jonn Axsen and George Beard and Nicolo Daina and Erik Figenbaum and Niklas Jakobsson and Patrick Jochem and Neale Kinnear and Patrick Plötz and Jose Pontes and Nazir Refa and Frances Sprei and Tom Turrentine and Bert Witkamp</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C18" s="2" t="inlineStr">
         <is>
           <t>https://www.sciencedirect.com/science/article/pii/S1361920918301330</t>
         </is>
       </c>
-      <c r="D18" t="n">
+      <c r="D18" s="2" t="n">
         <v>2018</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" s="2" t="inlineStr">
         <is>
           <t>Classification of cities in Bangladesh based on remote sensing derived spatial characteristics</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" s="2" t="inlineStr">
         <is>
           <t>Md Shahinoor Rahman and Hossain Mohiuddin and Abdulla-Al Kafy and Pintu Kumar Sheel and Liping Di</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C19" s="2" t="inlineStr">
         <is>
           <t>https://www.sciencedirect.com/science/article/pii/S2226585618301316</t>
         </is>
       </c>
-      <c r="D19" t="n">
+      <c r="D19" s="2" t="n">
         <v>2019</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20" s="2" t="inlineStr">
         <is>
           <t>Transport sustainability of Dhaka: A measure of ecological footprint and means for sustainable transportation system</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B20" s="2" t="inlineStr">
         <is>
           <t>SM Labib and Hossain Mohiuddin and Shahadat Shakil</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C20" s="2" t="inlineStr">
         <is>
           <t>https://papers.ssrn.com/sol3/papers.cfm?abstract_id=2514806</t>
         </is>
       </c>
-      <c r="D20" t="n">
+      <c r="D20" s="2" t="n">
         <v>2014</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="A21" s="2" t="inlineStr">
         <is>
           <t>High impact prioritization of bikeshare program investment to improve disadvantaged communities' access to jobs and essential services</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B21" s="2" t="inlineStr">
         <is>
           <t>Xiaodong Qian and Deb Niemeier</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C21" s="2" t="inlineStr">
         <is>
           <t>https://www.sciencedirect.com/science/article/pii/S0966692318305374</t>
         </is>
       </c>
-      <c r="D21" t="n">
+      <c r="D21" s="2" t="n">
         <v>2019</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22" s="2" t="inlineStr">
         <is>
           <t>Bikesharing, equity, and disadvantaged communities: A case study in Chicago</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B22" s="2" t="inlineStr">
         <is>
           <t>Xiaodong Qian and Miguel Jaller</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C22" s="2" t="inlineStr">
         <is>
           <t>https://www.sciencedirect.com/science/article/pii/S0965856420306479</t>
         </is>
       </c>
-      <c r="D22" t="n">
+      <c r="D22" s="2" t="n">
         <v>2020</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" s="2" t="inlineStr">
         <is>
           <t>Dimensions of conservation: Exploring differences among energy behaviors</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B23" s="2" t="inlineStr">
         <is>
           <t>Beth Karlin and Nora Davis and Angela Sanguinetti and Kristen Gamble and David Kirkby and Daniel Stokols</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C23" s="2" t="inlineStr">
         <is>
           <t>https://journals.sagepub.com/doi/abs/10.1177/0013916512467532</t>
         </is>
       </c>
-      <c r="D23" t="n">
+      <c r="D23" s="2" t="n">
         <v>2014</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24" s="2" t="inlineStr">
         <is>
           <t>Categories and functionality of smart home technology for energy management</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B24" s="2" t="inlineStr">
         <is>
           <t>Rebecca Ford and Marco Pritoni and Angela Sanguinetti and Beth Karlin</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C24" s="2" t="inlineStr">
         <is>
           <t>https://www.sciencedirect.com/science/article/pii/S0360132317303062</t>
         </is>
       </c>
-      <c r="D24" t="n">
+      <c r="D24" s="2" t="n">
         <v>2017</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" s="2" t="inlineStr">
         <is>
           <t>Why do people like bicycling? Modeling affect toward bicycling</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B25" s="2" t="inlineStr">
         <is>
           <t>Yan Xing and Jamey Volker and Susan Handy</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C25" s="2" t="inlineStr">
         <is>
           <t>https://www.sciencedirect.com/science/article/pii/S1369847817304941</t>
         </is>
       </c>
-      <c r="D25" t="n">
+      <c r="D25" s="2" t="n">
         <v>2018</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" s="2" t="inlineStr">
         <is>
           <t>Repurposing the paving: The case of surplus residential parking in Davis, CA</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B26" s="2" t="inlineStr">
         <is>
           <t>Calvin G Thigpen and Jamey MB Volker</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="C26" s="2" t="inlineStr">
         <is>
           <t>https://www.sciencedirect.com/science/article/pii/S0264275116307259</t>
         </is>
       </c>
-      <c r="D26" t="n">
+      <c r="D26" s="2" t="n">
         <v>2017</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" s="2" t="inlineStr">
         <is>
           <t>Bike sharing differences among Millennials, Gen Xers, and Baby Boomers: Lessons learnt from New York City’s bike share</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="B27" s="2" t="inlineStr">
         <is>
           <t>Kailai Wang and Gulsah Akar and Yu-Jen Chen</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C27" s="2" t="inlineStr">
         <is>
           <t>https://www.sciencedirect.com/science/article/pii/S0965856417306419</t>
         </is>
       </c>
-      <c r="D27" t="n">
+      <c r="D27" s="2" t="n">
         <v>2018</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="A28" s="2" t="inlineStr">
         <is>
           <t>Gender gap generators for bike share ridership: Evidence from Citi bike system in New York City</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B28" s="2" t="inlineStr">
         <is>
           <t>Kailai Wang and Gulsah Akar</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C28" s="2" t="inlineStr">
         <is>
           <t>https://www.sciencedirect.com/science/article/pii/S0966692318306045</t>
         </is>
       </c>
-      <c r="D28" t="n">
+      <c r="D28" s="2" t="n">
         <v>2019</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>Wind speed influence on phytoplankton bloom dynamics in the Southern Ocean Marginal Ice Zone</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="inlineStr">
+        <is>
+          <t>Dillon T Fitch and J Keith Moore</t>
+        </is>
+      </c>
+      <c r="C29" s="2" t="inlineStr">
+        <is>
+          <t>https://agupubs.onlinelibrary.wiley.com/doi/abs/10.1029/2006JC004061</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>Traffic stress and bicycling to elementary and junior high school: Evidence from Davis, California</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="inlineStr">
+        <is>
+          <t>Dillon Fitch and Calvin Thigpen and Susan Handy</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="inlineStr">
+        <is>
+          <t>https://www.sciencedirect.com/science/article/pii/S2214140516000098</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="inlineStr">
+        <is>
+          <t>Wind speed influence on phytoplankton bloom dynamics in the Southern Ocean Marginal Ice Zone</t>
+        </is>
+      </c>
+      <c r="B31" s="2" t="inlineStr">
+        <is>
+          <t>Dillon T Fitch and J Keith Moore</t>
+        </is>
+      </c>
+      <c r="C31" s="2" t="inlineStr">
+        <is>
+          <t>https://agupubs.onlinelibrary.wiley.com/doi/abs/10.1029/2006JC004061</t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="inlineStr">
+        <is>
+          <t>Traffic stress and bicycling to elementary and junior high school: Evidence from Davis, California</t>
+        </is>
+      </c>
+      <c r="B32" s="2" t="inlineStr">
+        <is>
+          <t>Dillon Fitch and Calvin Thigpen and Susan Handy</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="inlineStr">
+        <is>
+          <t>https://www.sciencedirect.com/science/article/pii/S2214140516000098</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="inlineStr">
+        <is>
+          <t>Wind speed influence on phytoplankton bloom dynamics in the Southern Ocean Marginal Ice Zone</t>
+        </is>
+      </c>
+      <c r="B33" s="2" t="inlineStr">
+        <is>
+          <t>Dillon T Fitch and J Keith Moore</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="inlineStr">
+        <is>
+          <t>https://agupubs.onlinelibrary.wiley.com/doi/abs/10.1029/2006JC004061</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="n">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="inlineStr">
+        <is>
+          <t>Traffic stress and bicycling to elementary and junior high school: Evidence from Davis, California</t>
+        </is>
+      </c>
+      <c r="B34" s="2" t="inlineStr">
+        <is>
+          <t>Dillon Fitch and Calvin Thigpen and Susan Handy</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="inlineStr">
+        <is>
+          <t>https://www.sciencedirect.com/science/article/pii/S2214140516000098</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="n">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="inlineStr">
+        <is>
+          <t>Wind speed influence on phytoplankton bloom dynamics in the Southern Ocean Marginal Ice Zone</t>
+        </is>
+      </c>
+      <c r="B35" s="2" t="inlineStr">
+        <is>
+          <t>Dillon T Fitch and J Keith Moore</t>
+        </is>
+      </c>
+      <c r="C35" s="2" t="inlineStr">
+        <is>
+          <t>https://agupubs.onlinelibrary.wiley.com/doi/abs/10.1029/2006JC004061</t>
+        </is>
+      </c>
+      <c r="D35" s="2" t="n">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="inlineStr">
+        <is>
+          <t>Traffic stress and bicycling to elementary and junior high school: Evidence from Davis, California</t>
+        </is>
+      </c>
+      <c r="B36" s="2" t="inlineStr">
+        <is>
+          <t>Dillon Fitch and Calvin Thigpen and Susan Handy</t>
+        </is>
+      </c>
+      <c r="C36" s="2" t="inlineStr">
+        <is>
+          <t>https://www.sciencedirect.com/science/article/pii/S2214140516000098</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="n">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="inlineStr">
+        <is>
+          <t>Wind speed influence on phytoplankton bloom dynamics in the Southern Ocean Marginal Ice Zone</t>
+        </is>
+      </c>
+      <c r="B37" s="2" t="inlineStr">
+        <is>
+          <t>Dillon T Fitch and J Keith Moore</t>
+        </is>
+      </c>
+      <c r="C37" s="2" t="inlineStr">
+        <is>
+          <t>https://agupubs.onlinelibrary.wiley.com/doi/abs/10.1029/2006JC004061</t>
+        </is>
+      </c>
+      <c r="D37" s="2" t="n">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="inlineStr">
+        <is>
+          <t>Traffic stress and bicycling to elementary and junior high school: Evidence from Davis, California</t>
+        </is>
+      </c>
+      <c r="B38" s="2" t="inlineStr">
+        <is>
+          <t>Dillon Fitch and Calvin Thigpen and Susan Handy</t>
+        </is>
+      </c>
+      <c r="C38" s="2" t="inlineStr">
+        <is>
+          <t>https://www.sciencedirect.com/science/article/pii/S2214140516000098</t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="n">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="inlineStr">
+        <is>
+          <t>Wind speed influence on phytoplankton bloom dynamics in the Southern Ocean Marginal Ice Zone</t>
+        </is>
+      </c>
+      <c r="B39" s="2" t="inlineStr">
+        <is>
+          <t>Dillon T Fitch and J Keith Moore</t>
+        </is>
+      </c>
+      <c r="C39" s="2" t="inlineStr">
+        <is>
+          <t>https://agupubs.onlinelibrary.wiley.com/doi/abs/10.1029/2006JC004061</t>
+        </is>
+      </c>
+      <c r="D39" s="2" t="n">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="inlineStr">
+        <is>
+          <t>Traffic stress and bicycling to elementary and junior high school: Evidence from Davis, California</t>
+        </is>
+      </c>
+      <c r="B40" s="2" t="inlineStr">
+        <is>
+          <t>Dillon Fitch and Calvin Thigpen and Susan Handy</t>
+        </is>
+      </c>
+      <c r="C40" s="2" t="inlineStr">
+        <is>
+          <t>https://www.sciencedirect.com/science/article/pii/S2214140516000098</t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="n">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="inlineStr">
+        <is>
+          <t>Wind speed influence on phytoplankton bloom dynamics in the Southern Ocean Marginal Ice Zone</t>
+        </is>
+      </c>
+      <c r="B41" s="2" t="inlineStr">
+        <is>
+          <t>Dillon T Fitch and J Keith Moore</t>
+        </is>
+      </c>
+      <c r="C41" s="2" t="inlineStr">
+        <is>
+          <t>https://agupubs.onlinelibrary.wiley.com/doi/abs/10.1029/2006JC004061</t>
+        </is>
+      </c>
+      <c r="D41" s="2" t="n">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="inlineStr">
+        <is>
+          <t>Traffic stress and bicycling to elementary and junior high school: Evidence from Davis, California</t>
+        </is>
+      </c>
+      <c r="B42" s="2" t="inlineStr">
+        <is>
+          <t>Dillon Fitch and Calvin Thigpen and Susan Handy</t>
+        </is>
+      </c>
+      <c r="C42" s="2" t="inlineStr">
+        <is>
+          <t>https://www.sciencedirect.com/science/article/pii/S2214140516000098</t>
+        </is>
+      </c>
+      <c r="D42" s="2" t="n">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Wind speed influence on phytoplankton bloom dynamics in the Southern Ocean Marginal Ice Zone</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Dillon T Fitch and J Keith Moore</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>https://agupubs.onlinelibrary.wiley.com/doi/abs/10.1029/2006JC004061</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Traffic stress and bicycling to elementary and junior high school: Evidence from Davis, California</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Dillon Fitch and Calvin Thigpen and Susan Handy</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>https://www.sciencedirect.com/science/article/pii/S2214140516000098</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>2015</v>
       </c>
     </row>
     <row r="1048576" ht="12.8" customHeight="1" s="3"/>

</xml_diff>

<commit_message>
- Excel formatting - Validation to check if publication exists - Record execution time
</commit_message>
<xml_diff>
--- a/output/publications.xlsx
+++ b/output/publications.xlsx
@@ -447,13 +447,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:D31"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="2:9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="86.98" customWidth="1" style="2" min="1" max="1"/>
     <col width="79.89" customWidth="1" style="2" min="2" max="2"/>
@@ -491,241 +491,47 @@
     <row r="4" ht="12.8" customHeight="1" s="3">
       <c r="D4" s="2" t="n"/>
     </row>
-    <row r="5" ht="12.8" customHeight="1" s="3">
-      <c r="D5" s="2" t="n"/>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Wind speed influence on phytoplankton bloom dynamics in the Southern Ocean Marginal Ice Zone</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Dillon T Fitch and J Keith Moore</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://agupubs.onlinelibrary.wiley.com/doi/abs/10.1029/2006JC004061</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>2007</v>
+      </c>
     </row>
-    <row r="6" ht="12.8" customHeight="1" s="3">
-      <c r="D6" s="2" t="n"/>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Traffic stress and bicycling to elementary and junior high school: Evidence from Davis, California</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Dillon Fitch and Calvin Thigpen and Susan Handy</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://www.sciencedirect.com/science/article/pii/S2214140516000098</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>2015</v>
+      </c>
     </row>
-    <row r="7" ht="12.8" customHeight="1" s="3">
-      <c r="D7" s="2" t="n"/>
-    </row>
-    <row r="8" ht="12.8" customHeight="1" s="3">
-      <c r="D8" s="2" t="n"/>
-    </row>
-    <row r="9" ht="12.8" customHeight="1" s="3">
-      <c r="D9" s="2" t="n"/>
-    </row>
-    <row r="10" ht="12.8" customHeight="1" s="3">
-      <c r="D10" s="2" t="n"/>
-    </row>
-    <row r="11" ht="12.8" customHeight="1" s="3">
-      <c r="D11" s="2" t="n"/>
-    </row>
-    <row r="12" ht="12.8" customHeight="1" s="3">
-      <c r="D12" s="2" t="n"/>
-    </row>
-    <row r="13" ht="12.8" customHeight="1" s="3">
-      <c r="D13" s="2" t="n"/>
-    </row>
-    <row r="14" ht="12.8" customHeight="1" s="3">
-      <c r="D14" s="2" t="n"/>
-    </row>
-    <row r="15" ht="12.8" customHeight="1" s="3">
-      <c r="D15" s="2" t="n"/>
-    </row>
-    <row r="16" ht="12.8" customHeight="1" s="3">
-      <c r="D16" s="2" t="n"/>
-    </row>
-    <row r="17" ht="12.8" customHeight="1" s="3">
-      <c r="D17" s="2" t="n"/>
-    </row>
-    <row r="18" ht="12.8" customHeight="1" s="3">
-      <c r="D18" s="2" t="n"/>
-    </row>
-    <row r="19" ht="12.8" customHeight="1" s="3">
-      <c r="D19" s="2" t="n"/>
-    </row>
-    <row r="20" ht="12.8" customHeight="1" s="3">
-      <c r="D20" s="2" t="n"/>
-    </row>
-    <row r="21" ht="12.8" customHeight="1" s="3">
-      <c r="D21" s="2" t="n"/>
-    </row>
-    <row r="22" ht="12.8" customHeight="1" s="3">
-      <c r="D22" s="2" t="n"/>
-    </row>
-    <row r="23" ht="12.8" customHeight="1" s="3">
-      <c r="D23" s="2" t="n"/>
-    </row>
-    <row r="24" ht="12.8" customHeight="1" s="3">
-      <c r="D24" s="2" t="n"/>
-    </row>
-    <row r="25" ht="12.8" customHeight="1" s="3">
-      <c r="D25" s="2" t="n"/>
-    </row>
-    <row r="26" ht="12.8" customHeight="1" s="3">
-      <c r="D26" s="2" t="n"/>
-    </row>
-    <row r="27" ht="12.8" customHeight="1" s="3">
-      <c r="D27" s="2" t="n"/>
-    </row>
-    <row r="28" ht="12.8" customHeight="1" s="3">
-      <c r="D28" s="2" t="n"/>
-    </row>
-    <row r="29" ht="12.8" customHeight="1" s="3">
-      <c r="D29" s="2" t="n"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="2" t="inlineStr">
-        <is>
-          <t>Wind speed influence on phytoplankton bloom dynamics in the Southern Ocean Marginal Ice Zone</t>
-        </is>
-      </c>
-      <c r="B30" s="2" t="inlineStr">
-        <is>
-          <t>Dillon T Fitch and J Keith Moore</t>
-        </is>
-      </c>
-      <c r="C30" s="2" t="inlineStr">
-        <is>
-          <t>https://agupubs.onlinelibrary.wiley.com/doi/abs/10.1029/2006JC004061</t>
-        </is>
-      </c>
-      <c r="D30" s="2" t="n">
-        <v>2007</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="2" t="inlineStr">
-        <is>
-          <t>Traffic stress and bicycling to elementary and junior high school: Evidence from Davis, California</t>
-        </is>
-      </c>
-      <c r="B31" s="2" t="inlineStr">
-        <is>
-          <t>Dillon Fitch and Calvin Thigpen and Susan Handy</t>
-        </is>
-      </c>
-      <c r="C31" s="2" t="inlineStr">
-        <is>
-          <t>https://www.sciencedirect.com/science/article/pii/S2214140516000098</t>
-        </is>
-      </c>
-      <c r="D31" s="2" t="n">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="2" t="inlineStr">
-        <is>
-          <t>Wind speed influence on phytoplankton bloom dynamics in the Southern Ocean Marginal Ice Zone</t>
-        </is>
-      </c>
-      <c r="B32" s="2" t="inlineStr">
-        <is>
-          <t>Dillon T Fitch and J Keith Moore</t>
-        </is>
-      </c>
-      <c r="C32" s="2" t="inlineStr">
-        <is>
-          <t>https://agupubs.onlinelibrary.wiley.com/doi/abs/10.1029/2006JC004061</t>
-        </is>
-      </c>
-      <c r="D32" s="2" t="n">
-        <v>2007</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="2" t="inlineStr">
-        <is>
-          <t>Traffic stress and bicycling to elementary and junior high school: Evidence from Davis, California</t>
-        </is>
-      </c>
-      <c r="B33" s="2" t="inlineStr">
-        <is>
-          <t>Dillon Fitch and Calvin Thigpen and Susan Handy</t>
-        </is>
-      </c>
-      <c r="C33" s="2" t="inlineStr">
-        <is>
-          <t>https://www.sciencedirect.com/science/article/pii/S2214140516000098</t>
-        </is>
-      </c>
-      <c r="D33" s="2" t="n">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="2" t="inlineStr">
-        <is>
-          <t>Wind speed influence on phytoplankton bloom dynamics in the Southern Ocean Marginal Ice Zone</t>
-        </is>
-      </c>
-      <c r="B34" s="2" t="inlineStr">
-        <is>
-          <t>Dillon T Fitch and J Keith Moore</t>
-        </is>
-      </c>
-      <c r="C34" s="2" t="inlineStr">
-        <is>
-          <t>https://agupubs.onlinelibrary.wiley.com/doi/abs/10.1029/2006JC004061</t>
-        </is>
-      </c>
-      <c r="D34" s="2" t="n">
-        <v>2007</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="2" t="inlineStr">
-        <is>
-          <t>Traffic stress and bicycling to elementary and junior high school: Evidence from Davis, California</t>
-        </is>
-      </c>
-      <c r="B35" s="2" t="inlineStr">
-        <is>
-          <t>Dillon Fitch and Calvin Thigpen and Susan Handy</t>
-        </is>
-      </c>
-      <c r="C35" s="2" t="inlineStr">
-        <is>
-          <t>https://www.sciencedirect.com/science/article/pii/S2214140516000098</t>
-        </is>
-      </c>
-      <c r="D35" s="2" t="n">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Wind speed influence on phytoplankton bloom dynamics in the Southern Ocean Marginal Ice Zone</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Dillon T Fitch and J Keith Moore</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>https://agupubs.onlinelibrary.wiley.com/doi/abs/10.1029/2006JC004061</t>
-        </is>
-      </c>
-      <c r="D36" t="n">
-        <v>2007</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Traffic stress and bicycling to elementary and junior high school: Evidence from Davis, California</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Dillon Fitch and Calvin Thigpen and Susan Handy</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>https://www.sciencedirect.com/science/article/pii/S2214140516000098</t>
-        </is>
-      </c>
-      <c r="D37" t="n">
-        <v>2015</v>
-      </c>
-    </row>
+    <row r="1048576" ht="12.8" customHeight="1" s="3"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>